<commit_message>
Converts CSV files to Excel files
</commit_message>
<xml_diff>
--- a/Attachments/Billing_Report_2020-07-10.xlsx
+++ b/Attachments/Billing_Report_2020-07-10.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,492 +356,328 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Servicer ID</t>
+          <t>Cert</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Lender Loan Number</t>
+          <t>Lender Loan #</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Certificate Number</t>
+          <t>City</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Borrower Name</t>
+          <t>State</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Property Address</t>
+          <t>Zip</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Original Effective Date</t>
+          <t>Orig Loan Amt</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Loan Amount</t>
+          <t>Orig Appr Value</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Billing Date</t>
+          <t>Orig Sales Price</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Invoice Number</t>
+          <t>Last Ins Amt</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Current Principal Balance</t>
+          <t>Renewal Period</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Billing Rate</t>
+          <t>Renewal Option</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Premium Due</t>
+          <t>Refund Ind</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Tax Rate</t>
+          <t>Cov %</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Tax Amount</t>
+          <t>Loan Closing Date</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Total Amount</t>
+          <t>Next Due Date</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>MI Paid By</t>
+          <t>Days Past Due</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16812-0001-0</t>
+          <t>3470039372</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>315232-437</t>
+          <t>329696-590</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19732096</t>
+          <t>PHOENIX</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Aherne, Brian</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
+          <t>85033</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>5/29/2008</t>
+          <t>87400</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>93500</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5/29/2020</t>
+          <t>92000</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>340064</t>
+          <t>87400</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>Zero Monthly</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>30</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>12/30/1998</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>01/01/2020</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Borrower</t>
+          <t>196</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16812-0001-0</t>
+          <t>3877345727</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>315232-437</t>
+          <t>0579129166</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>19732096</t>
+          <t>WATSONTOWN</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Aherne, Brian</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
+          <t>17777</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>5/29/2008</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>6/29/2020</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>342274</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>Zero Monthly</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>20</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>04/12/2007</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>05/01/2020</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Borrower</t>
+          <t>75</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16812-0001-0</t>
+          <t>6301710550</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>315232-437</t>
+          <t>0579130324</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>19732096</t>
+          <t>SPOKANE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Aherne, Brian</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
+          <t>99207</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>5/29/2008</t>
+          <t>113400</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>114000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>7/29/2020</t>
+          <t>113400</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>344454</t>
+          <t>113400</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>173900.0</t>
+          <t>Zero Monthly</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>C</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>R</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>10/11/2007</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>24.64</t>
+          <t>05/01/2020</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Borrower</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>16812-0001-0</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>7602359142</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>68441331</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Gross, Tracy</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1208 Williamsburg Drive - Champaign, IL 61821-0000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>9/1/2012</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>79705.0</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>6/1/2020</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>342274</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>71371.0</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0.64</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>42.51</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>42.51</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Borrower</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>16812-0001-0</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>7602359142</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>68441331</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Gross, Tracy</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1208 Williamsburg Drive - Champaign, IL 61821-0000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>9/1/2012</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>79705.0</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>7/1/2020</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>344454</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>71371.0</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>0.64</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>42.51</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>42.51</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Borrower</t>
+          <t>75</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correctly converts the CSV file to .xlsx file
</commit_message>
<xml_diff>
--- a/Attachments/Billing_Report_2020-07-10.xlsx
+++ b/Attachments/Billing_Report_2020-07-10.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,328 +356,492 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Cert</t>
+          <t>Servicer ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Lender Loan #</t>
+          <t>Lender Loan Number</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>Certificate Number</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>State</t>
+          <t>Borrower Name</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Zip</t>
+          <t>Property Address</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Orig Loan Amt</t>
+          <t>Original Effective Date</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Orig Appr Value</t>
+          <t>Loan Amount</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Orig Sales Price</t>
+          <t>Billing Date</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Last Ins Amt</t>
+          <t>Invoice Number</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Renewal Period</t>
+          <t>Current Principal Balance</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Renewal Option</t>
+          <t>Billing Rate</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Refund Ind</t>
+          <t>Premium Due</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Cov %</t>
+          <t>Tax Rate</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Loan Closing Date</t>
+          <t>Tax Amount</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Next Due Date</t>
+          <t>Total Amount</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Days Past Due</t>
+          <t>MI Paid By</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3470039372</t>
+          <t>16812-0001-0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>329696-590</t>
+          <t>315232-437</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PHOENIX</t>
+          <t>19732096</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>Aherne, Brian</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>85033</t>
+          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>87400</t>
+          <t>5/29/2008</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>93500</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>92000</t>
+          <t>5/29/2020</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>87400</t>
+          <t>340064</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Zero Monthly</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>12/30/1998</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>01/01/2020</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>196</t>
+          <t>Borrower</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3877345727</t>
+          <t>16812-0001-0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0579129166</t>
+          <t>315232-437</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>WATSONTOWN</t>
+          <t>19732096</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>Aherne, Brian</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17777</t>
+          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>5/29/2008</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>6/29/2020</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>80000</t>
+          <t>342274</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Zero Monthly</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>04/12/2007</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>05/01/2020</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>Borrower</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6301710550</t>
+          <t>16812-0001-0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0579130324</t>
+          <t>315232-437</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SPOKANE</t>
+          <t>19732096</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>Aherne, Brian</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>99207</t>
+          <t>199 Pine Grove Drive - Pittsfield, MA 01201-0000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>113400</t>
+          <t>5/29/2008</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>114000</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>113400</t>
+          <t>7/29/2020</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>113400</t>
+          <t>344454</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Zero Monthly</t>
+          <t>173900.0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>0.17</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>10/11/2007</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>05/01/2020</t>
+          <t>24.64</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>75</t>
+          <t>Borrower</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>16812-0001-0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7602359142</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>68441331</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Gross, Tracy</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1208 Williamsburg Drive - Champaign, IL 61821-0000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>9/1/2012</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>79705.0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>6/1/2020</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>342274</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>71371.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0.64</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>42.51</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>42.51</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Borrower</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>16812-0001-0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7602359142</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>68441331</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Gross, Tracy</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1208 Williamsburg Drive - Champaign, IL 61821-0000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9/1/2012</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>79705.0</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>7/1/2020</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>344454</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>71371.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.64</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>42.51</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>42.51</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Borrower</t>
         </is>
       </c>
     </row>

</xml_diff>